<commit_message>
add materials for session 10
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fedietri/GitHub/23-1-nmok/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B3ABE8-93CE-3449-BB42-48CA233751B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3185722E-6AFD-8942-9782-5C829E29C98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>week</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>exercises/e09.html</t>
+  </si>
+  <si>
+    <t>slides/slides.html#/session-10-systematization-what-constitutes-autonomy-in-digital-communication</t>
   </si>
 </sst>
 </file>
@@ -499,7 +502,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -702,6 +705,9 @@
       <c r="C11" t="s">
         <v>20</v>
       </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
       <c r="G11" t="s">
         <v>11</v>
       </c>

</xml_diff>